<commit_message>
File matching working accordingly
</commit_message>
<xml_diff>
--- a/output/Azienda.xlsx
+++ b/output/Azienda.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,12 +456,12 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Cliente</t>
+          <t>Società</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Indirizzo</t>
+          <t>Via</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -476,12 +476,12 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Provincia</t>
+          <t>Stato/Provincia</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>E-Mail</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
@@ -501,52 +501,52 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Partita IVA</t>
+          <t>Partita Iva</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Codice fiscale</t>
+          <t>Codice Fiscale</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Nome referente</t>
+          <t>Nome</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Cognome referente</t>
+          <t>Cognome</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Forma giuridica</t>
+          <t>Forma Giuridica</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Provenienza</t>
+          <t>Fonte del lead</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Km annui percorsi</t>
+          <t>Km Annui Percorsi</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Fatturato</t>
+          <t>Reddito annuale</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>GDPR</t>
+          <t>Consenso Privacy</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Consenso Promozioni e Newsletter</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
@@ -556,7 +556,47 @@
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Data creazione</t>
+          <t>Data Richiesta</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Extra Km</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Marca</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Modello</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Chilometri</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Durata</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Carburante</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Prezzo</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Anticipo</t>
         </is>
       </c>
     </row>
@@ -651,6 +691,46 @@
           <t>25/01/2024 14:14:37</t>
         </is>
       </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> €20 mese /15000 km</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Lynk &amp; Co</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Phev</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 30000</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 36</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Ibrida</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 420</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6000</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -741,6 +821,46 @@
       <c r="Y3" t="inlineStr">
         <is>
           <t>30/01/2024 09:23:39</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> €20 mese /20000 km</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Tesla</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Long range Model</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 40000</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 48</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Elettrica</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 689</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 6500</t>
         </is>
       </c>
     </row>
@@ -829,6 +949,46 @@
           <t>10/02/2024 18:49:17</t>
         </is>
       </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -922,6 +1082,46 @@
           <t>29/01/2024 21:59:07</t>
         </is>
       </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1013,6 +1213,42 @@
           <t>30/01/2024 10:57:42</t>
         </is>
       </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Audi</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 40 TDI 204CV Quattro S tronic A4 Allroad</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 48</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Diesel</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 555</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5000</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1104,6 +1340,42 @@
           <t>31/01/2024 13:38:49</t>
         </is>
       </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> €120 mese /60000 km</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> BMW</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> sDrive18d X3</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 30000</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Diesel</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 691</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1193,6 +1465,46 @@
       <c r="Y8" t="inlineStr">
         <is>
           <t>31/01/2024 15:48:33</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AB8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AF8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -1287,6 +1599,46 @@
           <t>01/02/2024 17:54:11</t>
         </is>
       </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> €90 mese /60000 km</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> DS Automobiles</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> BlueHDi 130</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 45000</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 36</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Diesel</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 476</t>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5000</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1379,6 +1731,42 @@
           <t>14/02/2024 18:28:52</t>
         </is>
       </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> €120 mese /60000 km</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> BMW</t>
+        </is>
+      </c>
+      <c r="AB10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> sDrive18d X3</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 30000</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Diesel</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 545</t>
+        </is>
+      </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5000</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1467,6 +1855,46 @@
           <t>10/01/2024 21:09:54</t>
         </is>
       </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> €20 mese /15000 km</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Alfa Romeo</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1.6 diesel</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 30000</t>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 36</t>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Diesel</t>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 412</t>
+        </is>
+      </c>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5000</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1567,6 +1995,46 @@
           <t>01/02/2024 15:15:41</t>
         </is>
       </c>
+      <c r="Z12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AA12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AB12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AD12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AE12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AF12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AG12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1667,6 +2135,46 @@
       <c r="Y13" t="inlineStr">
         <is>
           <t>20/02/2024 16:42:08</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>nan</t>
         </is>
       </c>
     </row>
@@ -1761,6 +2269,46 @@
           <t>01/02/2024 00:41:27</t>
         </is>
       </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> €20 mese /15000 km</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Audi</t>
+        </is>
+      </c>
+      <c r="AB14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 35 TDI S</t>
+        </is>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 45000</t>
+        </is>
+      </c>
+      <c r="AD14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 36</t>
+        </is>
+      </c>
+      <c r="AE14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Diesel</t>
+        </is>
+      </c>
+      <c r="AF14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 664</t>
+        </is>
+      </c>
+      <c r="AG14" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1852,6 +2400,46 @@
           <t>18/02/2024 14:51:45</t>
         </is>
       </c>
+      <c r="Z15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> €75 mese /80000 km</t>
+        </is>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> BMW</t>
+        </is>
+      </c>
+      <c r="AB15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 116d Busines Serie</t>
+        </is>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 40000</t>
+        </is>
+      </c>
+      <c r="AD15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 48</t>
+        </is>
+      </c>
+      <c r="AE15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Diesel</t>
+        </is>
+      </c>
+      <c r="AF15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 485</t>
+        </is>
+      </c>
+      <c r="AG15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>